<commit_message>
Tweak notes to reflect change to AMR components
</commit_message>
<xml_diff>
--- a/midas_manifest_v5.xlsx
+++ b/midas_manifest_v5.xlsx
@@ -93,9 +93,6 @@
     <t>Information about the source of the sample, e.g. BSAC ID</t>
   </si>
   <si>
-    <t>Comma-separated list of antibiotics to which the sampled organism displays resistance. Each antibiotic must be followed by the MIC, SIR and, optionally, the diagnostic centre. See notes.</t>
-  </si>
-  <si>
     <t>Condition of host. Must be one of "diseased", "healthy" or "carriage".</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>An internal identifier for the sample assigned by the depositing institute. Must be unique across all samples from a given institute, e.g. NHV0102000.</t>
+  </si>
+  <si>
+    <t>Comma-separated list of antibiotics to which the sampled organism displays resistance. Each antibiotic must be followed by the SIR and, optionally, the MIC, and the method used to determine the result. See notes.</t>
   </si>
 </sst>
 </file>
@@ -1390,13 +1390,13 @@
         <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>11</v>
@@ -1405,40 +1405,40 @@
         <v>12</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>21</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="P1" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>1</v>
@@ -32015,7 +32015,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>14</v>
@@ -32027,7 +32027,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -32059,7 +32059,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -32087,11 +32087,11 @@
     </row>
     <row r="5" spans="1:27" s="4" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -32123,7 +32123,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -32151,11 +32151,11 @@
     </row>
     <row r="8" spans="1:27" s="4" customFormat="1">
       <c r="A8" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -32215,7 +32215,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -32271,11 +32271,11 @@
     </row>
     <row r="12" spans="1:27" s="4" customFormat="1">
       <c r="A12" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -32363,10 +32363,10 @@
     </row>
     <row r="15" spans="1:27" s="4" customFormat="1">
       <c r="A15" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
@@ -32397,13 +32397,13 @@
     </row>
     <row r="16" spans="1:27" s="4" customFormat="1">
       <c r="A16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -32459,10 +32459,10 @@
     </row>
     <row r="18" spans="1:27" s="4" customFormat="1">
       <c r="A18" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -32523,13 +32523,13 @@
     </row>
     <row r="20" spans="1:27" s="4" customFormat="1">
       <c r="A20" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -32557,13 +32557,13 @@
     </row>
     <row r="21" spans="1:27" s="4" customFormat="1">
       <c r="A21" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -32591,10 +32591,10 @@
     </row>
     <row r="22" spans="1:27" s="4" customFormat="1">
       <c r="A22" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>20</v>
@@ -32625,13 +32625,13 @@
     </row>
     <row r="23" spans="1:27" s="4" customFormat="1">
       <c r="A23" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -32689,10 +32689,10 @@
     </row>
     <row r="25" spans="1:27" s="4" customFormat="1">
       <c r="A25" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>17</v>
@@ -32751,13 +32751,13 @@
     </row>
     <row r="27" spans="1:27" s="4" customFormat="1">
       <c r="A27" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -32849,7 +32849,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="1" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>

</xml_diff>